<commit_message>
Figured out single layer network with vertex attribute for color but still hard to see
</commit_message>
<xml_diff>
--- a/CurrentData/Raw Edgelists_Excel/SLR_Combined_VectorTypes.xlsx
+++ b/CurrentData/Raw Edgelists_Excel/SLR_Combined_VectorTypes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="71">
   <si>
     <t>Vector</t>
   </si>
@@ -225,6 +225,18 @@
   </si>
   <si>
     <t>Concern</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>#8FBC8F</t>
+  </si>
+  <si>
+    <t>#B22222</t>
+  </si>
+  <si>
+    <t>#DAA520</t>
   </si>
 </sst>
 </file>
@@ -542,524 +554,716 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>63</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>44</v>
       </c>
       <c r="B28" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>64</v>
       </c>
       <c r="B35" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="B42" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="B45" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
       <c r="B46" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
       <c r="B47" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
       <c r="B48" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
       <c r="B49" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
       <c r="B50" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
       <c r="B51" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
       <c r="B52" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
       <c r="B53" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
       <c r="B54" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
       <c r="B55" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
       <c r="B56" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
       <c r="B57" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
       <c r="B58" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
       <c r="B59" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
       <c r="B60" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
       <c r="B61" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
       <c r="B62" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
       <c r="B63" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
       <c r="B64" t="s">
         <v>66</v>
+      </c>
+      <c r="C64" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create edge colors and create second network for only edge weights >10 and no 0 degree vertices
</commit_message>
<xml_diff>
--- a/CurrentData/Raw Edgelists_Excel/SLR_Combined_VectorTypes.xlsx
+++ b/CurrentData/Raw Edgelists_Excel/SLR_Combined_VectorTypes.xlsx
@@ -125,9 +125,6 @@
     <t>Public Support</t>
   </si>
   <si>
-    <t>Don't Know</t>
-  </si>
-  <si>
     <t>Info Share/Use</t>
   </si>
   <si>
@@ -237,6 +234,9 @@
   </si>
   <si>
     <t>#DAA520</t>
+  </si>
+  <si>
+    <t>DK</t>
   </si>
 </sst>
 </file>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +570,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -581,7 +581,7 @@
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -592,7 +592,7 @@
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -603,7 +603,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -614,7 +614,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -625,7 +625,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -636,7 +636,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -647,7 +647,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -658,7 +658,7 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -669,7 +669,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -680,7 +680,7 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -691,7 +691,7 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -702,7 +702,7 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -713,7 +713,7 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
         <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -735,18 +735,18 @@
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -757,7 +757,7 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -768,7 +768,7 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -779,7 +779,7 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -790,7 +790,7 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -798,10 +798,10 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -809,10 +809,10 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -820,10 +820,10 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -831,10 +831,10 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -842,10 +842,10 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -853,21 +853,21 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -875,10 +875,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -886,10 +886,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -897,10 +897,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -908,10 +908,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -919,351 +919,351 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C55" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C57" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>